<commit_message>
Changes to generic model to simulate the heating load of several ERS models.
Generic models defined for:
ON80-89
ON70-79
PQ80-89
PQ70-79
BC80-89
BC70-79
AB80-89
AB70-79
ATL80-89 (Atlantic)
ATL70-79
MBSK80-89 (Manitoba and Saskatchewan)
MBSK70-79
</commit_message>
<xml_diff>
--- a/OptFramework/ERS 70-89 models.xlsx
+++ b/OptFramework/ERS 70-89 models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="9210" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="9210" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ON80-89" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,17 @@
     <sheet name="PQ70-79" sheetId="5" r:id="rId4"/>
     <sheet name="BC80-89" sheetId="7" r:id="rId5"/>
     <sheet name="BC70-79" sheetId="8" r:id="rId6"/>
+    <sheet name="AB70-79" sheetId="9" r:id="rId7"/>
+    <sheet name="AB80-89" sheetId="10" r:id="rId8"/>
+    <sheet name="ATL70-79" sheetId="11" r:id="rId9"/>
+    <sheet name="ATL80-89" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="81">
   <si>
     <t>window geometry calculations</t>
   </si>
@@ -1558,6 +1562,862 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>206.94</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <f>+(B26-B25)*(D31-D26)</f>
+        <v>44.836999999999996</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <f>+(C27-C26)*(D31-D27)</f>
+        <v>48.75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2">
+        <f>+C2/C3</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <f>+(B27-B28)*(D31-D28)</f>
+        <v>44.836999999999996</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <f>+(C28-C25)*(D32-D28)</f>
+        <v>48.75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <f>+(B30*C31)</f>
+        <v>206.94</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f>+C28*B27</f>
+        <v>206.94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="15">
+        <f>+H2*$C$5/100</f>
+        <v>6.7255499999999993</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="19">
+        <f>+H8/K8</f>
+        <v>4.1387999999999998</v>
+      </c>
+      <c r="K8" s="9">
+        <f>+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <f>+C3/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="16">
+        <f>+H3*$C$5/100</f>
+        <v>7.3125</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9" si="0">+H9/K9</f>
+        <v>4.5</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" ref="K9:K11" si="1">+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="24">
+        <f>2.1+C8</f>
+        <v>7.85</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="17">
+        <f>+H4*$C$5/100</f>
+        <v>6.7255499999999993</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="21">
+        <f>+H10/K10</f>
+        <v>4.1387999999999998</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="23">
+        <f>+C8-C7</f>
+        <v>3.75</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="18">
+        <f>+H5*$C$5/100</f>
+        <v>7.3125</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="22">
+        <f>+H11/K11</f>
+        <v>4.5</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+$D$34</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+$D$36</f>
+        <v>4.625</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+$B$33</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+$B$34</f>
+        <v>4.6387999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="10">
+        <f>+$C$37</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="16">
+        <f>+$C$38</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="17">
+        <f>+$B$41</f>
+        <v>13.295999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="17">
+        <f>+$B$42</f>
+        <v>9.1571999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="12">
+        <f>+$C$45</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="18">
+        <f>+$C$46</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4">
+        <f>+$C$4</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4">
+        <f>+$C$4</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C27" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D27" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D28" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f>+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B31" si="2">+$C$4</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:D32" si="3">+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C31" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="9">
+        <f>+B25+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="9">
+        <f>+C25</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.6387999999999998</v>
+      </c>
+      <c r="C34" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.6387999999999998</v>
+      </c>
+      <c r="C35" s="9">
+        <f>+C29</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <f>+D33+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9">
+        <f>+B33</f>
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="9">
+        <f>+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <f>+D34+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="20">
+        <f>+B26</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C26+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="11">
+        <f>+D26+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="20">
+        <f>+B27</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C38" s="11">
+        <f>+C37+J9</f>
+        <v>5</v>
+      </c>
+      <c r="D38" s="11">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="20">
+        <f>+B31</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C39" s="11">
+        <f>+C37+$J$9</f>
+        <v>5</v>
+      </c>
+      <c r="D39" s="11">
+        <f>+D37+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="20">
+        <f>+B30</f>
+        <v>13.795999999999999</v>
+      </c>
+      <c r="C40" s="11">
+        <f>+C30+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="11">
+        <f>+D38+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B27-0.5</f>
+        <v>13.295999999999999</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C27</f>
+        <v>15</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="21">
+        <f>+B41-$J$10</f>
+        <v>9.1571999999999996</v>
+      </c>
+      <c r="C42" s="7">
+        <f>+C28</f>
+        <v>15</v>
+      </c>
+      <c r="D42" s="7">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="21">
+        <f>+B42</f>
+        <v>9.1571999999999996</v>
+      </c>
+      <c r="C43" s="7">
+        <f>+C42</f>
+        <v>15</v>
+      </c>
+      <c r="D43" s="7">
+        <f>+D42+$K$10</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="21">
+        <f>+B41</f>
+        <v>13.295999999999999</v>
+      </c>
+      <c r="C44" s="7">
+        <f>+C43</f>
+        <v>15</v>
+      </c>
+      <c r="D44" s="7">
+        <f>+D43</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="14">
+        <f>+B28</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
+        <f>+C28-0.5</f>
+        <v>14.5</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="14">
+        <f>+B25</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="14">
+        <f>+C45-$J$11</f>
+        <v>10</v>
+      </c>
+      <c r="D46" s="14">
+        <f>+D25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="14">
+        <f>+B29</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="14">
+        <f>+C46</f>
+        <v>10</v>
+      </c>
+      <c r="D47" s="14">
+        <f>+D46+$K$11</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="14">
+        <f>+B32</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="14">
+        <f>+C45</f>
+        <v>14.5</v>
+      </c>
+      <c r="D48" s="14">
+        <f>+D47</f>
+        <v>4.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
@@ -4130,7 +4990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5836,4 +6696,2572 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>217.61</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <f>+(B26-B25)*(D31-D26)</f>
+        <v>47.148833333333336</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <f>+(C27-C26)*(D31-D27)</f>
+        <v>48.75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2">
+        <f>+C2/C3</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <f>+(B27-B28)*(D31-D28)</f>
+        <v>47.148833333333336</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <f>+(C28-C25)*(D32-D28)</f>
+        <v>48.75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <f>+(B30*C31)</f>
+        <v>217.61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f>+C28*B27</f>
+        <v>217.61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="15">
+        <f>+H2*$C$5/100</f>
+        <v>7.0723250000000011</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="19">
+        <f>+H8/K8</f>
+        <v>4.3522000000000007</v>
+      </c>
+      <c r="K8" s="9">
+        <f>+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <f>+C3/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="16">
+        <f>+H3*$C$5/100</f>
+        <v>7.3125</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9" si="0">+H9/K9</f>
+        <v>4.5</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" ref="K9:K11" si="1">+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="24">
+        <f>2.1+C8</f>
+        <v>7.85</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="17">
+        <f>+H4*$C$5/100</f>
+        <v>7.0723250000000011</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="21">
+        <f>+H10/K10</f>
+        <v>4.3522000000000007</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="23">
+        <f>+C8-C7</f>
+        <v>3.75</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="18">
+        <f>+H5*$C$5/100</f>
+        <v>7.3125</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="22">
+        <f>+H11/K11</f>
+        <v>4.5</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+$D$34</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+$D$36</f>
+        <v>4.625</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+$B$33</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+$B$34</f>
+        <v>4.8522000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="10">
+        <f>+$C$37</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="16">
+        <f>+$C$38</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="17">
+        <f>+$B$41</f>
+        <v>14.007333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="17">
+        <f>+$B$42</f>
+        <v>9.6551333333333318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="12">
+        <f>+$C$45</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="18">
+        <f>+$C$46</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4">
+        <f>+$C$4</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4">
+        <f>+$C$4</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C27" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D27" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D28" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f>+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B31" si="2">+$C$4</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:D32" si="3">+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C31" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>+$C$3</f>
+        <v>15</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="9">
+        <f>+B25+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="9">
+        <f>+C25</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.8522000000000007</v>
+      </c>
+      <c r="C34" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.8522000000000007</v>
+      </c>
+      <c r="C35" s="9">
+        <f>+C29</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <f>+D33+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9">
+        <f>+B33</f>
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="9">
+        <f>+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <f>+D34+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="20">
+        <f>+B26</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C26+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="11">
+        <f>+D26+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="20">
+        <f>+B27</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C38" s="11">
+        <f>+C37+J9</f>
+        <v>5</v>
+      </c>
+      <c r="D38" s="11">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="20">
+        <f>+B31</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C39" s="11">
+        <f>+C37+$J$9</f>
+        <v>5</v>
+      </c>
+      <c r="D39" s="11">
+        <f>+D37+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="20">
+        <f>+B30</f>
+        <v>14.507333333333333</v>
+      </c>
+      <c r="C40" s="11">
+        <f>+C30+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="11">
+        <f>+D38+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B27-0.5</f>
+        <v>14.007333333333333</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C27</f>
+        <v>15</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="21">
+        <f>+B41-$J$10</f>
+        <v>9.6551333333333318</v>
+      </c>
+      <c r="C42" s="7">
+        <f>+C28</f>
+        <v>15</v>
+      </c>
+      <c r="D42" s="7">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="21">
+        <f>+B42</f>
+        <v>9.6551333333333318</v>
+      </c>
+      <c r="C43" s="7">
+        <f>+C42</f>
+        <v>15</v>
+      </c>
+      <c r="D43" s="7">
+        <f>+D42+$K$10</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="21">
+        <f>+B41</f>
+        <v>14.007333333333333</v>
+      </c>
+      <c r="C44" s="7">
+        <f>+C43</f>
+        <v>15</v>
+      </c>
+      <c r="D44" s="7">
+        <f>+D43</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="14">
+        <f>+B28</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
+        <f>+C28-0.5</f>
+        <v>14.5</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="14">
+        <f>+B25</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="14">
+        <f>+C45-$J$11</f>
+        <v>10</v>
+      </c>
+      <c r="D46" s="14">
+        <f>+D25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="14">
+        <f>+B29</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="14">
+        <f>+C46</f>
+        <v>10</v>
+      </c>
+      <c r="D47" s="14">
+        <f>+D46+$K$11</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="14">
+        <f>+B32</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="14">
+        <f>+C45</f>
+        <v>14.5</v>
+      </c>
+      <c r="D48" s="14">
+        <f>+D47</f>
+        <v>4.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>252.52</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <f>+(B26-B25)*(D31-D26)</f>
+        <v>51.293125000000003</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <f>+(C27-C26)*(D31-D27)</f>
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2">
+        <f>+C2/C3</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <f>+(B27-B28)*(D31-D28)</f>
+        <v>51.293125000000003</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <f>+(C28-C25)*(D32-D28)</f>
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <f>+(B30*C31)</f>
+        <v>252.52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f>+C28*B27</f>
+        <v>252.52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="15">
+        <f>+H2*$C$5/100</f>
+        <v>7.6939687499999998</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="19">
+        <f>+H8/K8</f>
+        <v>4.73475</v>
+      </c>
+      <c r="K8" s="9">
+        <f>+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <f>+C3/2</f>
+        <v>8</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="16">
+        <f>+H3*$C$5/100</f>
+        <v>7.8</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9" si="0">+H9/K9</f>
+        <v>4.8</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" ref="K9:K11" si="1">+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="24">
+        <f>2.1+C8</f>
+        <v>7.85</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="17">
+        <f>+H4*$C$5/100</f>
+        <v>7.6939687499999998</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="21">
+        <f>+H10/K10</f>
+        <v>4.73475</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="23">
+        <f>+C8-C7</f>
+        <v>3.75</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="18">
+        <f>+H5*$C$5/100</f>
+        <v>7.8</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="22">
+        <f>+H11/K11</f>
+        <v>4.8</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+$D$34</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+$D$36</f>
+        <v>4.625</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+$B$33</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+$B$34</f>
+        <v>5.23475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="10">
+        <f>+$C$37</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="16">
+        <f>+$C$38</f>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="17">
+        <f>+$B$41</f>
+        <v>15.282500000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="17">
+        <f>+$B$42</f>
+        <v>10.547750000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="12">
+        <f>+$C$45</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="18">
+        <f>+$C$46</f>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4">
+        <f>+$C$4</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4">
+        <f>+$C$4</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C27" s="3">
+        <f>+$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="D27" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <f>+$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="D28" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f>+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B31" si="2">+$C$4</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:D32" si="3">+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C31" s="3">
+        <f>+$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>+$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="9">
+        <f>+B25+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="9">
+        <f>+C25</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="19">
+        <f>+B33+$J$8</f>
+        <v>5.23475</v>
+      </c>
+      <c r="C34" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="19">
+        <f>+B33+$J$8</f>
+        <v>5.23475</v>
+      </c>
+      <c r="C35" s="9">
+        <f>+C29</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <f>+D33+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9">
+        <f>+B33</f>
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="9">
+        <f>+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <f>+D34+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="20">
+        <f>+B26</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C26+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="11">
+        <f>+D26+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="20">
+        <f>+B27</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C38" s="11">
+        <f>+C37+J9</f>
+        <v>5.3</v>
+      </c>
+      <c r="D38" s="11">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="20">
+        <f>+B31</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C39" s="11">
+        <f>+C37+$J$9</f>
+        <v>5.3</v>
+      </c>
+      <c r="D39" s="11">
+        <f>+D37+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="20">
+        <f>+B30</f>
+        <v>15.782500000000001</v>
+      </c>
+      <c r="C40" s="11">
+        <f>+C30+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="11">
+        <f>+D38+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B27-0.5</f>
+        <v>15.282500000000001</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C27</f>
+        <v>16</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="21">
+        <f>+B41-$J$10</f>
+        <v>10.547750000000001</v>
+      </c>
+      <c r="C42" s="7">
+        <f>+C28</f>
+        <v>16</v>
+      </c>
+      <c r="D42" s="7">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="21">
+        <f>+B42</f>
+        <v>10.547750000000001</v>
+      </c>
+      <c r="C43" s="7">
+        <f>+C42</f>
+        <v>16</v>
+      </c>
+      <c r="D43" s="7">
+        <f>+D42+$K$10</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="21">
+        <f>+B41</f>
+        <v>15.282500000000001</v>
+      </c>
+      <c r="C44" s="7">
+        <f>+C43</f>
+        <v>16</v>
+      </c>
+      <c r="D44" s="7">
+        <f>+D43</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="14">
+        <f>+B28</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
+        <f>+C28-0.5</f>
+        <v>15.5</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="14">
+        <f>+B25</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="14">
+        <f>+C45-$J$11</f>
+        <v>10.7</v>
+      </c>
+      <c r="D46" s="14">
+        <f>+D25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="14">
+        <f>+B29</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="14">
+        <f>+C46</f>
+        <v>10.7</v>
+      </c>
+      <c r="D47" s="14">
+        <f>+D46+$K$11</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="14">
+        <f>+B32</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="14">
+        <f>+C45</f>
+        <v>15.5</v>
+      </c>
+      <c r="D48" s="14">
+        <f>+D47</f>
+        <v>4.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>193.07</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <f>+(B26-B25)*(D31-D26)</f>
+        <v>44.81982142857143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <f>+(C27-C26)*(D31-D27)</f>
+        <v>45.5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2">
+        <f>+C2/C3</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <f>+(B27-B28)*(D31-D28)</f>
+        <v>44.81982142857143</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <f>+(C28-C25)*(D32-D28)</f>
+        <v>45.5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <f>+(B30*C31)</f>
+        <v>193.07</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f>+C28*B27</f>
+        <v>193.07</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="15">
+        <f>+H2*$C$5/100</f>
+        <v>6.7229732142857141</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="19">
+        <f>+H8/K8</f>
+        <v>4.1372142857142853</v>
+      </c>
+      <c r="K8" s="9">
+        <f>+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <f>+C3/2</f>
+        <v>7</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="16">
+        <f>+H3*$C$5/100</f>
+        <v>6.8250000000000002</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9" si="0">+H9/K9</f>
+        <v>4.2</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" ref="K9:K11" si="1">+($C$8-$C$6)/2</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="24">
+        <f>2.1+C8</f>
+        <v>7.85</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="17">
+        <f>+H4*$C$5/100</f>
+        <v>6.7229732142857141</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="21">
+        <f>+H10/K10</f>
+        <v>4.1372142857142853</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="23">
+        <f>+C8-C7</f>
+        <v>3.75</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="18">
+        <f>+H5*$C$5/100</f>
+        <v>6.8250000000000002</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="22">
+        <f>+H11/K11</f>
+        <v>4.2</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="1"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+$D$34</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+$D$36</f>
+        <v>4.625</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+$B$33</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+$B$34</f>
+        <v>4.6372142857142853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="10">
+        <f>+$C$37</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="16">
+        <f>+$C$38</f>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="17">
+        <f>+$B$41</f>
+        <v>13.290714285714285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="17">
+        <f>+$B$42</f>
+        <v>9.1535000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="12">
+        <f>+$C$45</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="18">
+        <f>+$C$46</f>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4">
+        <f>+$C$4</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4">
+        <f>+$C$4</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C27" s="3">
+        <f>+$C$3</f>
+        <v>14</v>
+      </c>
+      <c r="D27" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <f>+$C$3</f>
+        <v>14</v>
+      </c>
+      <c r="D28" s="3">
+        <f>+$C$6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f>+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B31" si="2">+$C$4</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:D32" si="3">+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C31" s="3">
+        <f>+$C$3</f>
+        <v>14</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <f>+$C$3</f>
+        <v>14</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="9">
+        <f>+B25+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="9">
+        <f>+C25</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.6372142857142853</v>
+      </c>
+      <c r="C34" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <f>+$D$25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="19">
+        <f>+B33+$J$8</f>
+        <v>4.6372142857142853</v>
+      </c>
+      <c r="C35" s="9">
+        <f>+C29</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <f>+D33+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9">
+        <f>+B33</f>
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="9">
+        <f>+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <f>+D34+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="20">
+        <f>+B26</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C26+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="11">
+        <f>+D26+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="20">
+        <f>+B27</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C38" s="11">
+        <f>+C37+J9</f>
+        <v>4.7</v>
+      </c>
+      <c r="D38" s="11">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="20">
+        <f>+B31</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C39" s="11">
+        <f>+C37+$J$9</f>
+        <v>4.7</v>
+      </c>
+      <c r="D39" s="11">
+        <f>+D37+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="20">
+        <f>+B30</f>
+        <v>13.790714285714285</v>
+      </c>
+      <c r="C40" s="11">
+        <f>+C30+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="11">
+        <f>+D38+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B27-0.5</f>
+        <v>13.290714285714285</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C27</f>
+        <v>14</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D27+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="21">
+        <f>+B41-$J$10</f>
+        <v>9.1535000000000011</v>
+      </c>
+      <c r="C42" s="7">
+        <f>+C28</f>
+        <v>14</v>
+      </c>
+      <c r="D42" s="7">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="21">
+        <f>+B42</f>
+        <v>9.1535000000000011</v>
+      </c>
+      <c r="C43" s="7">
+        <f>+C42</f>
+        <v>14</v>
+      </c>
+      <c r="D43" s="7">
+        <f>+D42+$K$10</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="21">
+        <f>+B41</f>
+        <v>13.290714285714285</v>
+      </c>
+      <c r="C44" s="7">
+        <f>+C43</f>
+        <v>14</v>
+      </c>
+      <c r="D44" s="7">
+        <f>+D43</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="14">
+        <f>+B28</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
+        <f>+C28-0.5</f>
+        <v>13.5</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D28+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="14">
+        <f>+B25</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="14">
+        <f>+C45-$J$11</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D46" s="14">
+        <f>+D25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="14">
+        <f>+B29</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="14">
+        <f>+C46</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D47" s="14">
+        <f>+D46+$K$11</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="14">
+        <f>+B32</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="14">
+        <f>+C45</f>
+        <v>13.5</v>
+      </c>
+      <c r="D48" s="14">
+        <f>+D47</f>
+        <v>4.625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>